<commit_message>
Updated parser for final team
Proballers removed div id from tables.  Needs to be tested further.
</commit_message>
<xml_diff>
--- a/Data/aus_boomers_players.xlsx
+++ b/Data/aus_boomers_players.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Emanuel\DataScience\AusBoomers\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Emanuel\DataScience\AusBoomers\Tokyo2020\Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91B51F8-E1D5-460F-A050-5C6566E6AD01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A47A533-B032-4C61-8F9E-9FFDDACAE49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13005" yWindow="7470" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="53">
   <si>
     <t>SF</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>PF</t>
+  </si>
+  <si>
+    <t>Nathan Sobey</t>
+  </si>
+  <si>
+    <t>Selected</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -544,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,17 +568,18 @@
     <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -591,41 +601,44 @@
       <c r="G1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -647,41 +660,42 @@
       <c r="G2" s="7">
         <v>33721</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="7"/>
+      <c r="I2">
         <v>5</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>4.2</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>2.4</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>1.2</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>50</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>71.400000000000006</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>50</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>20.2</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>0.2</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -703,41 +717,42 @@
       <c r="G3" s="7">
         <v>35266</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="7"/>
+      <c r="I3">
         <v>242</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>16.3</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>8</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>56</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>10</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>60.1</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>56.1</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>20.100000000000001</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>27.2</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -759,41 +774,44 @@
       <c r="G4" s="7">
         <v>32366</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4">
         <v>698</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>8.9</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1.7</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>43.2</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>39</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>85.6</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>54.1</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>14.5</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>31.8</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -815,41 +833,44 @@
       <c r="G5" s="7">
         <v>31755</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="6">
         <v>494</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="6">
         <v>5.9</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="6">
         <v>4.5999999999999996</v>
       </c>
-      <c r="K5" s="6">
+      <c r="L5" s="6">
         <v>0.8</v>
       </c>
-      <c r="L5" s="6">
+      <c r="M5" s="6">
         <v>49</v>
       </c>
-      <c r="M5" s="6">
+      <c r="N5" s="6">
         <v>30.9</v>
       </c>
-      <c r="N5" s="6">
+      <c r="O5" s="6">
         <v>80</v>
       </c>
-      <c r="O5" s="6">
+      <c r="P5" s="6">
         <v>51</v>
       </c>
-      <c r="P5" s="6">
+      <c r="Q5" s="6">
         <v>13.8</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="R5" s="6">
         <v>19.399999999999999</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -868,41 +889,44 @@
       <c r="G6" s="7">
         <v>32052</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6">
         <v>503</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>8.5</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>3.2</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>3.7</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>45.1</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>41</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>76.099999999999994</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>58</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>12.7</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>30.7</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -924,41 +948,42 @@
       <c r="G7" s="7">
         <v>35486</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="7"/>
+      <c r="I7">
         <v>263</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>2.8</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>0.6</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>43.5</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>32.700000000000003</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>68</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>50.2</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>12</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>6.6</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -977,41 +1002,42 @@
       <c r="G8" s="7">
         <v>33108</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="7"/>
+      <c r="I8" s="4">
         <v>59</v>
       </c>
-      <c r="I8" s="6">
+      <c r="J8" s="6">
         <v>4</v>
       </c>
-      <c r="J8" s="6">
+      <c r="K8" s="6">
         <v>1.8</v>
       </c>
-      <c r="K8" s="6">
+      <c r="L8" s="6">
         <v>0.6</v>
       </c>
-      <c r="L8" s="6">
+      <c r="M8" s="6">
         <v>42.7</v>
       </c>
-      <c r="M8" s="6">
+      <c r="N8" s="6">
         <v>40.299999999999997</v>
       </c>
-      <c r="N8" s="6">
+      <c r="O8" s="6">
         <v>81.5</v>
       </c>
-      <c r="O8" s="6">
+      <c r="P8" s="6">
         <v>58.4</v>
       </c>
-      <c r="P8" s="6">
+      <c r="Q8" s="6">
         <v>11.4</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="R8" s="6">
         <v>1.2</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1030,41 +1056,44 @@
       <c r="G9" s="7">
         <v>33124</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9">
         <v>434</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>5.6</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>1.8</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>3.7</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>38.9</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>36.799999999999997</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>83.8</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>47.9</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>9.8000000000000007</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>10.1</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1084,41 +1113,44 @@
       <c r="G10" s="7">
         <v>35493</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10">
         <v>91</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>4.3</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>1.5</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>41.4</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>34</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>58.5</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>51.6</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>9.8000000000000007</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>3.1</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1140,41 +1172,44 @@
       <c r="G11" s="7">
         <v>34893</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="2">
         <v>245</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>5.7</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>1.8</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>2.1</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>40.700000000000003</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>30.5</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>76.400000000000006</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>47.3</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>8.3000000000000007</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>3.1</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1196,41 +1231,44 @@
       <c r="G12" s="7">
         <v>36846</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12">
         <v>17</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>2.5</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>2.2999999999999998</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>0.6</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>47.2</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>16.7</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>54.5</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>50</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>6.4</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>0</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1252,41 +1290,42 @@
       <c r="G13" s="7">
         <v>35800</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="7"/>
+      <c r="I13" s="1">
         <v>5</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>3</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>0</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>28.6</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>27.3</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>0</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>35.700000000000003</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>3.4</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>-0.1</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1308,41 +1347,42 @@
       <c r="G14" s="7">
         <v>35462</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="7"/>
+      <c r="I14" s="3">
         <v>19</v>
       </c>
-      <c r="I14" s="4">
+      <c r="J14" s="4">
         <v>1.7</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K14" s="3">
         <v>1</v>
       </c>
-      <c r="K14" s="4">
+      <c r="L14" s="4">
         <v>0.3</v>
       </c>
-      <c r="L14" s="3">
+      <c r="M14" s="3">
         <v>30.6</v>
       </c>
-      <c r="M14" s="4">
+      <c r="N14" s="4">
         <v>26.1</v>
       </c>
-      <c r="N14" s="4">
+      <c r="O14" s="4">
         <v>100</v>
       </c>
-      <c r="O14" s="4">
+      <c r="P14" s="4">
         <v>38.9</v>
       </c>
-      <c r="P14" s="3">
+      <c r="Q14" s="3">
         <v>2.7</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="R14" s="4">
         <v>-0.2</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1361,8 +1401,11 @@
       <c r="G15" s="7">
         <v>32440</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H15" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1378,9 +1421,12 @@
       <c r="G16" s="7">
         <v>33819</v>
       </c>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1396,8 +1442,11 @@
       <c r="G17" s="7">
         <v>34997</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1413,9 +1462,10 @@
       <c r="G18" s="7">
         <v>33785</v>
       </c>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="7"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1437,8 +1487,9 @@
       <c r="G19" s="7">
         <v>35898</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1460,9 +1511,10 @@
       <c r="G20" s="7">
         <v>35956</v>
       </c>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="7"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1484,8 +1536,9 @@
       <c r="G21" s="7">
         <v>33162</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1501,8 +1554,9 @@
       <c r="G22" s="7">
         <v>34060</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1518,8 +1572,11 @@
       <c r="G23" s="7">
         <v>35242</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1535,8 +1592,9 @@
       <c r="G24" s="7">
         <v>34930</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -1552,10 +1610,33 @@
       <c r="G25" s="7">
         <v>37539</v>
       </c>
+      <c r="H25" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>65681</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26">
+        <v>193</v>
+      </c>
+      <c r="G26" s="7">
+        <v>33068</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R14">
-    <sortCondition descending="1" ref="P2:P14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S14">
+    <sortCondition descending="1" ref="Q2:Q14"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Tokyo 2020 comparison
Added Olympic stats and compared with historical efficiency
</commit_message>
<xml_diff>
--- a/Data/aus_boomers_players.xlsx
+++ b/Data/aus_boomers_players.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Emanuel\DataScience\AusBoomers\Tokyo2020\Team\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Emanuel\DataScience\AusBoomers\Tokyo2020\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A47A533-B032-4C61-8F9E-9FFDDACAE49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86845B55-821B-4A55-B269-5FCDF05EFF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="4200" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="53">
   <si>
     <t>SF</t>
   </si>
@@ -556,7 +556,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,9 +1610,7 @@
       <c r="G25" s="7">
         <v>37539</v>
       </c>
-      <c r="H25" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">

</xml_diff>